<commit_message>
Bug fix - config reading was missing one item. Also updated .csv and .xlsx files
</commit_message>
<xml_diff>
--- a/Migration/SQLServer/1_TranslateTableDDLs/SourceToTargetTablesConfig.xlsx
+++ b/Migration/SQLServer/1_TranslateTableDDLs/SourceToTargetTablesConfig.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git-Repos\AzureSynapseScriptsAndAccelerators\Migration\SQLServer\1_TranslateTableDDLs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Migration\SQLServer\modules\1_TranslateTableDDLs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC63CFA-9B76-4C99-92B5-EEF20C4B6678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D779863F-B257-445D-B4C1-1F0609CD6875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{6E24CC37-2027-4639-A45A-A26BB2FFCBF2}"/>
+    <workbookView xWindow="0" yWindow="2715" windowWidth="28770" windowHeight="15750" xr2:uid="{6E24CC37-2027-4639-A45A-A26BB2FFCBF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -193,6 +193,9 @@
     <t>DimProduct</t>
   </si>
   <si>
+    <t>gailzsqlpool</t>
+  </si>
+  <si>
     <t>FactInternetSalesMkeys</t>
   </si>
   <si>
@@ -200,9 +203,6 @@
   </si>
   <si>
     <t>OrderDateKey|ProductKey|ShipDateKey</t>
-  </si>
-  <si>
-    <t>yourSQLPoolDbName</t>
   </si>
 </sst>
 </file>
@@ -218,7 +218,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -228,6 +228,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -244,10 +256,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -564,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E599576C-D4BE-467C-A95F-C1003D82894A}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27:J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,7 +642,7 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
         <v>40</v>
@@ -660,7 +674,7 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E3" t="s">
         <v>40</v>
@@ -692,7 +706,7 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E4" t="s">
         <v>40</v>
@@ -724,7 +738,7 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E5" t="s">
         <v>40</v>
@@ -756,7 +770,7 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E6" t="s">
         <v>40</v>
@@ -788,7 +802,7 @@
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E7" t="s">
         <v>40</v>
@@ -820,7 +834,7 @@
         <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E8" t="s">
         <v>40</v>
@@ -852,7 +866,7 @@
         <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E9" t="s">
         <v>40</v>
@@ -884,7 +898,7 @@
         <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E10" t="s">
         <v>40</v>
@@ -916,7 +930,7 @@
         <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E11" t="s">
         <v>40</v>
@@ -948,7 +962,7 @@
         <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E12" t="s">
         <v>40</v>
@@ -980,7 +994,7 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E13" t="s">
         <v>40</v>
@@ -1012,7 +1026,7 @@
         <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E14" t="s">
         <v>40</v>
@@ -1044,7 +1058,7 @@
         <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E15" t="s">
         <v>40</v>
@@ -1076,7 +1090,7 @@
         <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E16" t="s">
         <v>40</v>
@@ -1108,7 +1122,7 @@
         <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E17" t="s">
         <v>40</v>
@@ -1140,7 +1154,7 @@
         <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E18" t="s">
         <v>40</v>
@@ -1172,7 +1186,7 @@
         <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E19" t="s">
         <v>40</v>
@@ -1207,7 +1221,7 @@
         <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E20" t="s">
         <v>40</v>
@@ -1242,7 +1256,7 @@
         <v>12</v>
       </c>
       <c r="D21" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E21" t="s">
         <v>40</v>
@@ -1277,13 +1291,13 @@
         <v>12</v>
       </c>
       <c r="D22" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E22" t="s">
         <v>40</v>
       </c>
       <c r="F22" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G22" t="s">
         <v>13</v>
@@ -1297,8 +1311,8 @@
       <c r="J22" t="s">
         <v>42</v>
       </c>
-      <c r="K22" t="s">
-        <v>54</v>
+      <c r="K22" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1312,7 +1326,7 @@
         <v>12</v>
       </c>
       <c r="D23" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E23" t="s">
         <v>40</v>
@@ -1347,7 +1361,7 @@
         <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E24" t="s">
         <v>40</v>
@@ -1381,8 +1395,8 @@
       <c r="C25" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D25" t="s">
-        <v>55</v>
+      <c r="D25" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>40</v>
@@ -1416,8 +1430,8 @@
       <c r="C26" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D26" t="s">
-        <v>55</v>
+      <c r="D26" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>40</v>
@@ -1452,7 +1466,7 @@
         <v>12</v>
       </c>
       <c r="D27" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E27" t="s">
         <v>40</v>
@@ -1466,11 +1480,11 @@
       <c r="H27" t="s">
         <v>14</v>
       </c>
-      <c r="I27" t="s">
-        <v>39</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>53</v>
+      <c r="I27" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Re-organized item list in two functions for alignment with .csv and .xlsx config files.
</commit_message>
<xml_diff>
--- a/Migration/SQLServer/1_TranslateTableDDLs/SourceToTargetTablesConfig.xlsx
+++ b/Migration/SQLServer/1_TranslateTableDDLs/SourceToTargetTablesConfig.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Migration\SQLServer\modules\1_TranslateTableDDLs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git-Repos\AzureSynapseScriptsAndAccelerators\Migration\SQLServer\1_TranslateTableDDLs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D779863F-B257-445D-B4C1-1F0609CD6875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B38541F1-4FC0-480C-B558-08ED5B990702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2715" windowWidth="28770" windowHeight="15750" xr2:uid="{6E24CC37-2027-4639-A45A-A26BB2FFCBF2}"/>
+    <workbookView xWindow="14303" yWindow="2355" windowWidth="24495" windowHeight="15945" xr2:uid="{6E24CC37-2027-4639-A45A-A26BB2FFCBF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -193,9 +193,6 @@
     <t>DimProduct</t>
   </si>
   <si>
-    <t>gailzsqlpool</t>
-  </si>
-  <si>
     <t>FactInternetSalesMkeys</t>
   </si>
   <si>
@@ -203,6 +200,9 @@
   </si>
   <si>
     <t>OrderDateKey|ProductKey|ShipDateKey</t>
+  </si>
+  <si>
+    <t>yourSynapseSQLPoolDbName</t>
   </si>
 </sst>
 </file>
@@ -579,7 +579,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27:J27"/>
+      <selection activeCell="D3" sqref="D3:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,7 +642,7 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E2" t="s">
         <v>40</v>
@@ -674,7 +674,7 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s">
         <v>40</v>
@@ -706,7 +706,7 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E4" t="s">
         <v>40</v>
@@ -738,7 +738,7 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E5" t="s">
         <v>40</v>
@@ -770,7 +770,7 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E6" t="s">
         <v>40</v>
@@ -802,7 +802,7 @@
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E7" t="s">
         <v>40</v>
@@ -834,7 +834,7 @@
         <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E8" t="s">
         <v>40</v>
@@ -866,7 +866,7 @@
         <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E9" t="s">
         <v>40</v>
@@ -898,7 +898,7 @@
         <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E10" t="s">
         <v>40</v>
@@ -930,7 +930,7 @@
         <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E11" t="s">
         <v>40</v>
@@ -962,7 +962,7 @@
         <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E12" t="s">
         <v>40</v>
@@ -994,7 +994,7 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E13" t="s">
         <v>40</v>
@@ -1026,7 +1026,7 @@
         <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E14" t="s">
         <v>40</v>
@@ -1058,7 +1058,7 @@
         <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E15" t="s">
         <v>40</v>
@@ -1090,7 +1090,7 @@
         <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E16" t="s">
         <v>40</v>
@@ -1122,7 +1122,7 @@
         <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E17" t="s">
         <v>40</v>
@@ -1154,7 +1154,7 @@
         <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E18" t="s">
         <v>40</v>
@@ -1186,7 +1186,7 @@
         <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E19" t="s">
         <v>40</v>
@@ -1221,7 +1221,7 @@
         <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E20" t="s">
         <v>40</v>
@@ -1256,7 +1256,7 @@
         <v>12</v>
       </c>
       <c r="D21" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E21" t="s">
         <v>40</v>
@@ -1291,13 +1291,13 @@
         <v>12</v>
       </c>
       <c r="D22" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" t="s">
         <v>52</v>
-      </c>
-      <c r="E22" t="s">
-        <v>40</v>
-      </c>
-      <c r="F22" t="s">
-        <v>53</v>
       </c>
       <c r="G22" t="s">
         <v>13</v>
@@ -1312,7 +1312,7 @@
         <v>42</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1326,7 +1326,7 @@
         <v>12</v>
       </c>
       <c r="D23" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E23" t="s">
         <v>40</v>
@@ -1361,7 +1361,7 @@
         <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E24" t="s">
         <v>40</v>
@@ -1395,8 +1395,8 @@
       <c r="C25" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>52</v>
+      <c r="D25" t="s">
+        <v>55</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>40</v>
@@ -1430,8 +1430,8 @@
       <c r="C26" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>52</v>
+      <c r="D26" t="s">
+        <v>55</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>40</v>
@@ -1466,7 +1466,7 @@
         <v>12</v>
       </c>
       <c r="D27" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E27" t="s">
         <v>40</v>
@@ -1481,7 +1481,7 @@
         <v>14</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J27" s="4" t="s">
         <v>15</v>

</xml_diff>